<commit_message>
Overlap correction and unified interface for display control
Add the functionality of overlap corrections for pollyxt_tau. Meanwhile,
unified the interface for controlling the x-y-z range of all the plots.
In my understanding, this should be a big update. Be careful!
</commit_message>
<xml_diff>
--- a/doc/polly_overviews.xlsx
+++ b/doc/polly_overviews.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baars\AppData\Local\Temp\moz_mapi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zpyin\Desktop\Pollynet_Processing_Chain\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B9E60E-652F-4B18-8508-D0878562F257}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -200,7 +207,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -343,9 +350,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Eingabe" xfId="2" builtinId="20"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="输入" xfId="2" builtinId="20"/>
+    <cellStyle name="适中" xfId="1" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -622,30 +629,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M43" sqref="M43"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="9" style="2" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" style="3" customWidth="1"/>
-    <col min="7" max="8" width="19.85546875" style="3" customWidth="1"/>
-    <col min="9" max="10" width="18.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="4"/>
+    <col min="5" max="5" width="13.7265625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" style="3" customWidth="1"/>
+    <col min="7" max="8" width="19.81640625" style="3" customWidth="1"/>
+    <col min="9" max="10" width="18.1796875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="22.81640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="18.1796875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -686,7 +693,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
@@ -724,7 +731,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14"/>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
@@ -738,7 +745,7 @@
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>18</v>
       </c>
@@ -767,7 +774,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>19</v>
       </c>
@@ -796,7 +803,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="16" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
@@ -812,7 +819,7 @@
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>355</v>
       </c>
@@ -853,7 +860,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>27</v>
       </c>
@@ -894,7 +901,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>387</v>
       </c>
@@ -935,7 +942,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>407</v>
       </c>
@@ -976,7 +983,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>532</v>
       </c>
@@ -1017,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>28</v>
       </c>
@@ -1058,7 +1065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>607</v>
       </c>
@@ -1099,7 +1106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>1064</v>
       </c>
@@ -1138,7 +1145,7 @@
       </c>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>29</v>
       </c>
@@ -1177,7 +1184,7 @@
       </c>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>30</v>
       </c>
@@ -1216,7 +1223,7 @@
       </c>
       <c r="M16" s="7"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>31</v>
       </c>
@@ -1255,7 +1262,7 @@
       </c>
       <c r="M17" s="7"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>32</v>
       </c>
@@ -1294,7 +1301,7 @@
       </c>
       <c r="M18" s="7"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>37</v>
       </c>
@@ -1335,7 +1342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>38</v>
       </c>
@@ -1376,7 +1383,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="16" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
         <v>44</v>
       </c>
@@ -1392,7 +1399,7 @@
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>39</v>
       </c>
@@ -1437,7 +1444,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>40</v>
       </c>
@@ -1483,7 +1490,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>41</v>
       </c>
@@ -1526,7 +1533,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>42</v>
       </c>
@@ -1570,7 +1577,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>43</v>
       </c>
@@ -1615,7 +1622,7 @@
         <v>0.92592592592592582</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>45</v>
       </c>
@@ -1659,7 +1666,7 @@
         <v>2015.73</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>46</v>
       </c>
@@ -1702,7 +1709,7 @@
         <v>0.63873275421563613</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>47</v>
       </c>
@@ -1746,7 +1753,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
         <v>49</v>
       </c>
@@ -1788,7 +1795,7 @@
         <v>4.8842434306925855E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>50</v>
       </c>
@@ -1829,13 +1836,13 @@
         <v>2.0175999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="12"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="12"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
         <v>52</v>
       </c>
@@ -1865,7 +1872,7 @@
         <v>1.5228426395939101E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
         <v>53</v>
       </c>
@@ -1893,7 +1900,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="12"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -1903,7 +1910,7 @@
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="12"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -1913,7 +1920,7 @@
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>54</v>
       </c>
@@ -1955,7 +1962,7 @@
         <v>3.8461538461538519E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>55</v>
       </c>
@@ -1994,7 +2001,7 @@
         <v>-0.99900829560724536</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
@@ -2008,7 +2015,7 @@
       <c r="L40" s="10"/>
       <c r="M40" s="11"/>
     </row>
-    <row r="41" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="14" t="s">
         <v>56</v>
       </c>
@@ -2024,7 +2031,7 @@
       <c r="K41" s="15"/>
       <c r="L41" s="15"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B42" s="2">
         <v>1500</v>
       </c>

</xml_diff>